<commit_message>
fix: removes unnecessary scripts
</commit_message>
<xml_diff>
--- a/itens_processados.xlsx
+++ b/itens_processados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,12 +471,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nistatina Suspensão Oral</t>
+          <t>Nistatina 100.000 Unidades Internacionais/ml Suspensão Oral</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Medicamento, Material Odontológico, Hospitalar e Ambulatorial</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -501,12 +501,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nistanina</t>
+          <t>Nistanina 25.000 Ui/g Creme Vaginal</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Medicamento</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -531,12 +531,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nistatina + Óxido De Zinco</t>
+          <t>Nistatina + Oxido De Zinco 60grs</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Medicamento</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -561,12 +561,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Nimesulida</t>
+          <t>Nimesulida Gts 15 Ml</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Medicamento</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -591,27 +591,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Nimegon Met</t>
+          <t>Nimesulida 100 Mg Cx C/ 12 Comp</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Medicamento</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Medicamento</t>
+          <t>Medicamento, Material Odontológico, Hospitalar e Ambulatorial</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>UND</t>
+          <t>CAP</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['NIMEGON MET 50/850 56 CPRS']</t>
+          <t>['NIMESULIDA 100 MG CX C/ 12 COMP']</t>
         </is>
       </c>
     </row>
@@ -621,17 +621,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Nifedipino</t>
+          <t>Nimegon Met 50/850 56 Cprs</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Outros Materiais Permanentes</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Outros Materiais Permanentes</t>
+          <t>Medicamento</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>['NIFEDIPINO 20MG C/450']</t>
+          <t>['NIMEGON MET 50/850 56 CPRS']</t>
         </is>
       </c>
     </row>
@@ -651,17 +651,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nimegon</t>
+          <t>Nifedipino 20mg C/450</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Medicamento</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Medicamento</t>
+          <t>Outros Materiais Permanentes</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>['NIMEGON 50 MG']</t>
+          <t>['NIFEDIPINO 20MG C/450']</t>
         </is>
       </c>
     </row>
@@ -681,17 +681,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Nicho De Parede</t>
+          <t>Nimegon 50 Mg</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Móveis e Utensílios</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Móveis e Utensílios</t>
+          <t>Medicamento</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>['NINCHO DE PAREDE']</t>
+          <t>['NIMEGON 50 MG']</t>
         </is>
       </c>
     </row>
@@ -711,12 +711,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Fórmula Infantil</t>
+          <t>Nimesulida 100mg</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Outros Materiais Permanentes</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -731,7 +731,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>['NESTOGENO 2LT 800GRS']</t>
+          <t>['NIMESULIDA 100MG']</t>
         </is>
       </c>
     </row>
@@ -741,17 +741,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Neovangy</t>
+          <t>Nimesulida Gts 15 Ml (gen)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Outros Materiais Permanentes</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Outros Materiais Permanentes</t>
+          <t>Medicamento, Material Odontológico, Hospitalar e Ambulatorial</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -761,7 +761,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>['NEOVANGY 35 MG']</t>
+          <t>['NIMESULIDA GTS 15 ML (GEN)']</t>
         </is>
       </c>
     </row>
@@ -771,17 +771,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Minesol Corp Rosto Fps 70</t>
+          <t>Nincho De Parede</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Medicamento</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Medicamento</t>
+          <t>Móveis e Utensílios</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>['NEOSTRATA MINESOL CORP ROSTO FPS 70 120 ML']</t>
+          <t>['NINCHO DE PAREDE']</t>
         </is>
       </c>
     </row>
@@ -801,12 +801,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Neostar Minesol</t>
+          <t>Nimesulida Gel 40 Grs</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Outros Materiais Permanentes</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -821,57 +821,57 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>['NEOSTRA MINESOL']</t>
+          <t>['NIMESULIDA GEL 40 GRS']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>25012</v>
+        <v>25013</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Neozine</t>
+          <t>Nimesulida 50mg/ml Solução Oral</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Outros Materiais Permanentes</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Outros Materiais Permanentes</t>
+          <t>Medicamento, Material Odontológico, Hospitalar e Ambulatorial</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>UND</t>
+          <t>FRC</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>['NEOZINE 100MG 20CPRS']</t>
+          <t>['NIMESULIDA 50MG/ML SOLUÇÃO ORAL\t']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>25013</v>
+        <v>25014</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Neolefrin Xp</t>
+          <t>Nestogeno 2lt 800grs</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Medicamento</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Medicamento</t>
+          <t>Outros Materiais Permanentes</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -881,22 +881,22 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>['NEOLEFRIN XP 60 ML']</t>
+          <t>['NESTOGENO 2LT 800GRS']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>25014</v>
+        <v>25015</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Neoloratadina</t>
+          <t>Neovangy 35 Mg</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Outros Materiais Permanentes</t>
+          <t>não classificado</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -911,37 +911,1507 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>['NEOLORATADINA 12 COMP']</t>
+          <t>['NEOVANGY 35 MG']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>25015</v>
+        <v>25017</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>Neostrata Minesol Corp Rosto Fps 70 120 Ml</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>['NEOSTRATA MINESOL CORP ROSTO FPS 70 120 ML']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>25018</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Neostra Minesol</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>['NEOSTRA MINESOL']</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>25020</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Neovangy Mr 35 Mg</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>['NEOVANGY MR 35 MG']</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>25021</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Neozine 100mg 20cprs</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>['NEOZINE 100MG 20CPRS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>25022</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Neozine 25 Mg</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>['NEOZINE 25 MG']</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>25023</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Neozine 100 Mg 20 Cprs</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Medicamento, Material Odontológico, Hospitalar e Ambulatorial</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>['NEOZINE 100 MG 20 CPRS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>25025</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Neovangy Mr 35 Mg 60 Cp</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>['NEOVANGY MR 35 MG 60 CP']</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>25026</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Neolefrin Xp 60 Ml</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>['NEOLEFRIN XP 60 ML']</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>25027</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Neoloratadina 12 Comp</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>['NEOLORATADINA 12 COMP']</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25028</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Neofresh Col 15 Ml</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Medicamento, Material Odontológico, Hospitalar e Ambulatorial</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>['NEOFRESH COL 15 ML']</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>25029</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Neofolico 5 Mg 20 Cprs</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>['NEOFOLICO 5 MG 20 CPRS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>25030</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>Neofresh</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>['NEOFRESH']</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>25031</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Neomicina</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>['NEOMICINA']</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>25032</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Neosoro 30ml</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Aparelhos, Equipamentos, Utensílios Médico-odontológico, Laboratorial e Hospitalar</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>['NEOSORO 30ML']</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>25033</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Neosoro H 3 60 Ml</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>['NEOSORO H 3 60 ML']</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>25034</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Neosil Attack C/ 30 Cprs</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>['NEOSIL ATTACK C/ 30 CPRS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>25035</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Neomicina Bacitracina Pom 15 Mg</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>['NEOMICINA BACITRACINA POM 15 MG']</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>25036</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Neosemid 40mg</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>['NEOSEMID 40MG']</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>25037</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Nesina Pio 25/30 Mg</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>['NESINA PIO 25/30 MG']</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>25039</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Nesina Pio 25/15 Mg C/ 30 Cprs</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>['NESINA PIO 25/15 MG C/ 30 CPRS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>25040</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Nesina Met 12,5/1000 C/ 60 Comp</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>['NESINA MET 12,5/1000 C/ 60 COMP']</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>25041</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Nesina Met 12,5/850 60 Cprs</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>['NESINA MET 12,5/850 60 CPRS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>25042</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Neslac Supreme</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>['NESLAC SUPREME']</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>25043</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Nestogeno 2 - Fórmula Infantil,</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Gêneros Alimentícios</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LA</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>['NESTOGENO 2 - FÓRMULA INFANTIL,']</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>25044</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Nestogeno 2 400gr</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>['NESTOGENO 2 400GR']</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>25045</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Nestogeno 1 400 Gs</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>['NESTOGENO 1 400 GS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>25046</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Nessina Met 12.5/850</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>['NESSINA MET 12.5/850']</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>25047</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Nestogeno 1 - Formula Infantil</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Gêneros Alimentícios</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LA</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>['NESTOGENO 1 - FORMULA INFANTIL']</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>25048</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Neozine Gts 4 20ml (c1)**</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>['NEOZINE GTS 4 20ML (C1)**']</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>25049</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Nesina 25 Mg 30 Cprs</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
         <is>
           <t>Medicamento, Material Odontológico, Hospitalar e Ambulatorial</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>['NESINA 25 MG 30 CPRS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>25050</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Neozine Gts 4 20ml</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>['NEOZINE GTS 4 20ML']</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>25051</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Neozine 25 Mg 20 Cprs</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
         <is>
           <t>Medicamento, Material Odontológico, Hospitalar e Ambulatorial</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>UND</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>['NEOFRESH COL 15 ML']</t>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>['NEOZINE 25 MG 20 CPRS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>25052</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Neozine Gts 4 20 Ml (c1)</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Medicamento, Material Odontológico, Hospitalar e Ambulatorial</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>['NEOZINE GTS 4 20 ML (C1)']</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>25053</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Nesina 25 Mg 30 Cprs*</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Medicamento, Material Odontológico, Hospitalar e Ambulatorial</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>['NESINA 25 MG 30 CPRS*']</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>25054</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Nesina 25mg 30cprs</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>CX</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>['NESINA 25MG 30CPRS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>25055</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Nesina Met 12,5/1000</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>['NESINA MET 12,5/1000']</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>25056</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Nesina 25mg 30 Cprs</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>['NESINA 25MG 30 CPRS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>25057</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Nesina 25 Mg C/30comp</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>['NESINA 25 MG C/30COMP']</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>25058</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Nesina 25mg</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>['NESINA 25MG']</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>25059</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Noripurim 30cprs</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>['NORIPURIM 30CPRS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>25060</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Noripurum 30 Cprs Mast</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>['NORIPURUM 30 CPRS MAST']</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>25061</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Norifer Gotas Fr C/30ml</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>['NORIFER GOTAS FR C/30ML']</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>25062</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Noretisterona-estradiol 50-5mg Por Ml</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>['NORETISTERONA-ESTRADIOL 50-5MG POR ML']</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>25063</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Norfloxacino 400mg C/14 Cprs</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>['NORFLOXACINO 400MG C/14 CPRS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>25064</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Noripurum 30cprs</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>['NORIPURUM 30CPRS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>25065</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Nortriptilina 25 Mg 30 Comp</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Medicamento, Material Odontológico, Hospitalar e Ambulatorial</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>['NORTRIPTILINA 25 MG 30 COMP']</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>25066</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Nortriptilina 25mg</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>['NORTRIPTILINA 25MG']</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>25067</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Noripurum Iv 5 Amp 5 Ml</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Medicamento</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>['NORIPURUM IV 5 AMP 5 ML']</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>25068</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Noripurum Folico 30 Comp</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Medicamento, Material Odontológico, Hospitalar e Ambulatorial</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>CAP</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>['NORIPURUM FOLICO 30 COMP']</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>25069</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Noripurum Folico 30 Cprs</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>não classificado</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Outros Materiais Permanentes</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>['NORIPURUM FOLICO 30 CPRS']</t>
         </is>
       </c>
     </row>

</xml_diff>